<commit_message>
add test case with peer review comment
</commit_message>
<xml_diff>
--- a/DesignAndExecution/Caso de Prueba Pet_Store Remake.xlsx
+++ b/DesignAndExecution/Caso de Prueba Pet_Store Remake.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ismael\Desktop\Tecnologia\SpeedUp Tech\Repositorios Pet-Store\Repositorio Miguel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA127B7C-299B-4A03-9470-75CC6075B908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E382DB-9F81-4CE8-95B0-F9984C995553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="15396" windowHeight="8952" xr2:uid="{0D95BB56-36A7-45B8-A04F-19D58170236C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{0D95BB56-36A7-45B8-A04F-19D58170236C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="102">
   <si>
     <t>CP17</t>
   </si>
@@ -407,6 +405,12 @@
   <si>
     <t xml:space="preserve">1. Abrir postman                                                                     2. Agregar una request                                               3. Seleccionar el método DELET                                Ingresar el path/pet                   
 4. No ingresar id                                                              5. Enviar la request.                                                   </t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>No tiene URL por lo tanto no se puede probar el caso de prueba</t>
   </si>
 </sst>
 </file>
@@ -450,7 +454,7 @@
       <name val="Poppins"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,6 +470,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -514,13 +524,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,25 +853,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B0FBD1-B631-48F4-BAB3-AE7DA2B3E52C}">
   <dimension ref="B1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" customWidth="1"/>
-    <col min="5" max="5" width="34.44140625" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" customWidth="1"/>
-    <col min="7" max="7" width="32.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="11" max="11" width="0.5546875" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="34.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" customWidth="1"/>
+    <col min="7" max="7" width="32.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="0.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="19.8" x14ac:dyDescent="0.7">
+    <row r="1" spans="2:10" ht="19.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
@@ -880,8 +897,11 @@
       <c r="I1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -889,9 +909,10 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="2:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="2:10" ht="315" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
@@ -916,8 +937,11 @@
       <c r="I3" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" ht="217.8" x14ac:dyDescent="0.3">
+      <c r="J3" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="214.5" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -942,8 +966,11 @@
       <c r="I4" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" ht="217.8" x14ac:dyDescent="0.3">
+      <c r="J4" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="214.5" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -968,8 +995,11 @@
       <c r="I5" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" ht="217.8" x14ac:dyDescent="0.3">
+      <c r="J5" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="195" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
@@ -994,8 +1024,11 @@
       <c r="I6" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" ht="217.8" x14ac:dyDescent="0.3">
+      <c r="J6" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="195" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
@@ -1020,8 +1053,11 @@
       <c r="I7" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1031,7 +1067,7 @@
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="2:9" ht="365.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="393.75" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
@@ -1056,8 +1092,11 @@
       <c r="I9" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" ht="138.6" x14ac:dyDescent="0.3">
+      <c r="J9" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>32</v>
       </c>
@@ -1082,8 +1121,11 @@
       <c r="I10" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" ht="138.6" x14ac:dyDescent="0.3">
+      <c r="J10" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
@@ -1108,8 +1150,11 @@
       <c r="I11" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" ht="138.6" x14ac:dyDescent="0.3">
+      <c r="J11" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>38</v>
       </c>
@@ -1134,8 +1179,11 @@
       <c r="I12" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" ht="138.6" x14ac:dyDescent="0.3">
+      <c r="J12" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>40</v>
       </c>
@@ -1160,8 +1208,11 @@
       <c r="I13" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1171,7 +1222,7 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="2:9" ht="365.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="393.75" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>43</v>
       </c>
@@ -1196,8 +1247,11 @@
       <c r="I15" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="J15" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="156" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>46</v>
       </c>
@@ -1222,8 +1276,11 @@
       <c r="I16" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="J16" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="156" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>48</v>
       </c>
@@ -1248,8 +1305,11 @@
       <c r="I17" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="J17" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="117" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>49</v>
       </c>
@@ -1274,8 +1334,11 @@
       <c r="I18" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1285,7 +1348,7 @@
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
     </row>
-    <row r="20" spans="2:9" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
         <v>92</v>
       </c>
@@ -1310,8 +1373,11 @@
       <c r="I20" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" ht="138.6" x14ac:dyDescent="0.3">
+      <c r="J20" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>93</v>
       </c>
@@ -1336,8 +1402,11 @@
       <c r="I21" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" ht="138.6" x14ac:dyDescent="0.3">
+      <c r="J21" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="136.5" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>0</v>
       </c>
@@ -1362,8 +1431,11 @@
       <c r="I22" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="J22" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="117" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>3</v>
       </c>
@@ -1388,8 +1460,14 @@
       <c r="I23" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="J23" s="9" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I2:J2"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" sqref="I1 I3:I7 I9:I13 I20:I23 I15:I18" xr:uid="{44757228-372C-4BB5-9829-835694A888E0}">

</xml_diff>